<commit_message>
1. Clean configuration template for integration with KMD data models 2. Divide model initialization into read_config() and apply_model_extensions()
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_Automation_paper_1space_1v_1h_0c.xlsx
+++ b/twin4build/test/data/configuration_template_Automation_paper_1space_1v_1h_0c.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="6_{BFA7A2FF-EE31-474C-9095-512E26FEE44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83774CC6-4743-441C-8C9D-17FEA0BFA3F0}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="6_{BFA7A2FF-EE31-474C-9095-512E26FEE44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3E090D3-DA91-42DE-8F08-894E6EC56E5A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="9" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="3" r:id="rId1"/>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EEF019-D7A4-42FF-B5C0-3702855A99F7}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,12 +838,12 @@
         <v>77</v>
       </c>
       <c r="D2">
-        <f>IF(C2="T", 0.05, IF(C2="C", -0.01, ""))</f>
+        <f>IF(C2="T", 0.05, IF(C2="C", -0.5, ""))</f>
         <v>0.05</v>
       </c>
       <c r="E2">
-        <f>IF(C2="T", 0.1, IF(C2="C", 0, ""))</f>
-        <v>0.1</v>
+        <f>IF(C2="T", 0.8, IF(C2="C", 0, ""))</f>
+        <v>0.8</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2" si="0">IF(C2="T", 0, IF(C2="C", 0, ""))</f>
@@ -58232,7 +58232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A142E3-535E-45D7-B544-7DE9118FD57D}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -64286,7 +64286,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>